<commit_message>
Write code for dietary individual foood
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yumin's Thinkpad\Desktop\Read-Meat-Consumption---All-Cause-Mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D3055D-F084-4667-AF58-16FDF1F5B079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD976E10-DA8F-492D-8EDA-04335E980012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="333">
   <si>
     <t>Variables names</t>
   </si>
@@ -1006,6 +1006,66 @@
   </si>
   <si>
     <t>[During the past month], how often did {you/SP} eat any kind of cheese? Include cheese as a snack, cheese on burgers, sandwiches, and cheese mixed into such foods as lasagna, quesadillas, or casseroles. {Please do not count cheese on pizza.}[You can tell me per day, per week or per month.]</t>
+  </si>
+  <si>
+    <t>fped_dr1tot_0910.sas7bdat</t>
+  </si>
+  <si>
+    <t>PF_SEAFD_HI and PF_SEAFD_LOW</t>
+  </si>
+  <si>
+    <t>oz. eq</t>
+  </si>
+  <si>
+    <t>F_TOTAL</t>
+  </si>
+  <si>
+    <t>cup eq.</t>
+  </si>
+  <si>
+    <t>V_TOTAL</t>
+  </si>
+  <si>
+    <t>PF_MEAT</t>
+  </si>
+  <si>
+    <t>oz. eq.</t>
+  </si>
+  <si>
+    <t>V_LEGUMES</t>
+  </si>
+  <si>
+    <t>D_TOTAL</t>
+  </si>
+  <si>
+    <t>PF_CUREDMEAT</t>
+  </si>
+  <si>
+    <t>G_WHOLE</t>
+  </si>
+  <si>
+    <t>(oz. eq.)</t>
+  </si>
+  <si>
+    <t>D_CHEESE</t>
+  </si>
+  <si>
+    <t>PF_POULT</t>
+  </si>
+  <si>
+    <t>PF_NUTSDS</t>
+  </si>
+  <si>
+    <t>oz. eq.)</t>
+  </si>
+  <si>
+    <t>PF_EGGS</t>
+  </si>
+  <si>
+    <t>PF_MPS_TOTAL</t>
+  </si>
+  <si>
+    <t>(oz. eq.</t>
   </si>
 </sst>
 </file>
@@ -1361,7 +1421,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2165,10 +2225,13 @@
         <v>11</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>293</v>
+        <v>314</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>315</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>232</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -2215,13 +2278,13 @@
         <v>15</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2241,10 +2304,13 @@
         <v>14</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>292</v>
+        <v>318</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>317</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2264,13 +2330,13 @@
         <v>7</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>298</v>
+        <v>319</v>
+      </c>
+      <c r="G37" t="s">
+        <v>320</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2290,13 +2356,13 @@
         <v>6</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2316,13 +2382,13 @@
         <v>6</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2342,13 +2408,13 @@
         <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2368,13 +2434,13 @@
         <v>4</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2394,13 +2460,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2420,13 +2480,7 @@
         <v>3</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2441,10 +2495,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2464,13 +2515,13 @@
         <v>2</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3046,7 +3097,13 @@
         <v>8</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>294</v>
+        <v>327</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3066,7 +3123,13 @@
         <v>5</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>294</v>
+        <v>328</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3086,7 +3149,13 @@
         <v>5</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>294</v>
+        <v>330</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3106,7 +3175,13 @@
         <v>4</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>307</v>
+        <v>331</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3208,10 +3283,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CAA67E9-9811-4B5E-A7FC-26E0B3853EB9}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3673,6 +3748,452 @@
         <v>281</v>
       </c>
     </row>
+    <row r="30" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="3">
+        <v>15</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="3">
+        <v>14</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="3">
+        <v>7</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="3">
+        <v>6</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="3">
+        <v>6</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="3">
+        <v>4</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="3">
+        <v>3</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="3">
+        <v>2</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="3">
+        <v>11</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="3">
+        <v>8</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="3">
+        <v>5</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="3">
+        <v>5</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="3">
+        <v>4</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished replacing 7,9 with NA
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yumin's Thinkpad\Desktop\Read-Meat-Consumption---All-Cause-Mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33CA946-F317-4A4A-AD44-8E9DC4005A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E57637-A3CE-4BB5-8F10-2F38C1144428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1420,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
complete ounce to gram
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yumin's Thinkpad\Desktop\Read-Meat-Consumption---All-Cause-Mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218C1258-2C3D-420E-9B71-12842BDACC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6214A00F-0100-4CE9-AD35-1E45CBA10B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>